<commit_message>
Added missing NIR data for 2016
</commit_message>
<xml_diff>
--- a/R/input/GP 2016.xlsx
+++ b/R/input/GP 2016.xlsx
@@ -1,16 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26501"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FBFE3FC-123E-4E1B-97CC-CCEDCB5FF26D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="38290" yWindow="-21740" windowWidth="21820" windowHeight="37900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Spring Canola" sheetId="1" r:id="rId1"/>
     <sheet name="Winter Wheat" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1226,7 +1240,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1487,18 +1501,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1507,7 +1521,7 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1516,62 +1530,59 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1579,7 +1590,7 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1600,9 +1611,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1640,9 +1651,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1677,7 +1688,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1712,7 +1723,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1885,32 +1896,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:HU274"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="15" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="31.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.3828125" style="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="33.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="67.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.69140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.84375" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.84375" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.15234375" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.84375" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.15234375" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.84375" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.3828125" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="33.15234375" style="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="67.53515625" style="10" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="1" style="10" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="10"/>
+    <col min="14" max="16384" width="9.15234375" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1923,23 +1934,23 @@
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="1:13" s="2" customFormat="1" ht="61.5" x14ac:dyDescent="0.85">
-      <c r="A2" s="31" t="s">
+    <row r="2" spans="1:13" s="2" customFormat="1" ht="61.75" x14ac:dyDescent="1.5">
+      <c r="A2" s="30" t="s">
         <v>394</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
       <c r="L2" s="3"/>
     </row>
-    <row r="3" spans="1:13" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="1.05">
+    <row r="3" spans="1:13" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="1.75">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1953,7 +1964,7 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:13" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1967,7 +1978,7 @@
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="1:13" s="7" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" s="7" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
@@ -2006,7 +2017,7 @@
       </c>
       <c r="M5" s="6"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" s="26" t="s">
         <v>10</v>
       </c>
@@ -2037,7 +2048,7 @@
       <c r="L6" s="8"/>
       <c r="M6" s="9"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" s="27" t="s">
         <v>11</v>
       </c>
@@ -2063,7 +2074,7 @@
       </c>
       <c r="M7" s="9"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" s="26" t="s">
         <v>12</v>
       </c>
@@ -2094,7 +2105,7 @@
       <c r="L8" s="8"/>
       <c r="M8" s="9"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" s="27" t="s">
         <v>13</v>
       </c>
@@ -2120,7 +2131,7 @@
       </c>
       <c r="M9" s="9"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" s="26" t="s">
         <v>14</v>
       </c>
@@ -2151,7 +2162,7 @@
       <c r="L10" s="8"/>
       <c r="M10" s="9"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11" s="27" t="s">
         <v>15</v>
       </c>
@@ -2177,7 +2188,7 @@
       </c>
       <c r="M11" s="9"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" s="26" t="s">
         <v>16</v>
       </c>
@@ -2208,7 +2219,7 @@
       <c r="L12" s="8"/>
       <c r="M12" s="9"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13" s="27" t="s">
         <v>17</v>
       </c>
@@ -2234,7 +2245,7 @@
       </c>
       <c r="M13" s="9"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14" s="26" t="s">
         <v>18</v>
       </c>
@@ -2267,7 +2278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15" s="27" t="s">
         <v>19</v>
       </c>
@@ -2293,7 +2304,7 @@
       </c>
       <c r="M15" s="9"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16" s="26" t="s">
         <v>20</v>
       </c>
@@ -2324,7 +2335,7 @@
       <c r="L16" s="8"/>
       <c r="M16" s="9"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17" s="27" t="s">
         <v>21</v>
       </c>
@@ -2350,7 +2361,7 @@
       </c>
       <c r="M17" s="9"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A18" s="26" t="s">
         <v>22</v>
       </c>
@@ -2383,7 +2394,7 @@
       </c>
       <c r="M18" s="9"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A19" s="27" t="s">
         <v>23</v>
       </c>
@@ -2409,7 +2420,7 @@
       </c>
       <c r="M19" s="9"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A20" s="26" t="s">
         <v>24</v>
       </c>
@@ -2440,7 +2451,7 @@
       </c>
       <c r="M20" s="9"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A21" s="27" t="s">
         <v>25</v>
       </c>
@@ -2466,7 +2477,7 @@
       </c>
       <c r="M21" s="9"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A22" s="26" t="s">
         <v>26</v>
       </c>
@@ -2497,7 +2508,7 @@
       <c r="L22" s="8"/>
       <c r="M22" s="9"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A23" s="27" t="s">
         <v>27</v>
       </c>
@@ -2523,7 +2534,7 @@
       </c>
       <c r="M23" s="9"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A24" s="26" t="s">
         <v>28</v>
       </c>
@@ -2554,7 +2565,7 @@
       <c r="L24" s="8"/>
       <c r="M24" s="9"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A25" s="27" t="s">
         <v>29</v>
       </c>
@@ -2580,7 +2591,7 @@
       </c>
       <c r="M25" s="9"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A26" s="26" t="s">
         <v>30</v>
       </c>
@@ -2611,7 +2622,7 @@
       <c r="L26" s="8"/>
       <c r="M26" s="9"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A27" s="27" t="s">
         <v>31</v>
       </c>
@@ -2637,7 +2648,7 @@
       </c>
       <c r="M27" s="9"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A28" s="26" t="s">
         <v>32</v>
       </c>
@@ -2668,7 +2679,7 @@
       <c r="L28" s="8"/>
       <c r="M28" s="9"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A29" s="27" t="s">
         <v>33</v>
       </c>
@@ -2694,7 +2705,7 @@
       </c>
       <c r="M29" s="9"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A30" s="26" t="s">
         <v>34</v>
       </c>
@@ -2725,7 +2736,7 @@
       <c r="L30" s="8"/>
       <c r="M30" s="9"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A31" s="27" t="s">
         <v>35</v>
       </c>
@@ -2751,7 +2762,7 @@
       </c>
       <c r="M31" s="9"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A32" s="26" t="s">
         <v>36</v>
       </c>
@@ -2782,7 +2793,7 @@
       <c r="L32" s="8"/>
       <c r="M32" s="9"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A33" s="27" t="s">
         <v>37</v>
       </c>
@@ -2808,7 +2819,7 @@
       </c>
       <c r="M33" s="9"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A34" s="26" t="s">
         <v>38</v>
       </c>
@@ -2839,7 +2850,7 @@
       <c r="L34" s="8"/>
       <c r="M34" s="9"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A35" s="27" t="s">
         <v>39</v>
       </c>
@@ -2865,7 +2876,7 @@
       </c>
       <c r="M35" s="9"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A36" s="26" t="s">
         <v>40</v>
       </c>
@@ -2896,7 +2907,7 @@
       <c r="L36" s="8"/>
       <c r="M36" s="9"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A37" s="27" t="s">
         <v>41</v>
       </c>
@@ -2922,7 +2933,7 @@
       </c>
       <c r="M37" s="9"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A38" s="26" t="s">
         <v>42</v>
       </c>
@@ -2953,7 +2964,7 @@
       <c r="L38" s="8"/>
       <c r="M38" s="9"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A39" s="27" t="s">
         <v>43</v>
       </c>
@@ -2979,7 +2990,7 @@
       </c>
       <c r="M39" s="9"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A40" s="26" t="s">
         <v>44</v>
       </c>
@@ -3010,7 +3021,7 @@
       <c r="L40" s="8"/>
       <c r="M40" s="9"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A41" s="27" t="s">
         <v>45</v>
       </c>
@@ -3036,7 +3047,7 @@
       </c>
       <c r="M41" s="9"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A42" s="26" t="s">
         <v>46</v>
       </c>
@@ -3069,7 +3080,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A43" s="27" t="s">
         <v>48</v>
       </c>
@@ -3097,7 +3108,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A44" s="26" t="s">
         <v>49</v>
       </c>
@@ -3128,7 +3139,7 @@
       <c r="L44" s="8"/>
       <c r="M44" s="9"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A45" s="27" t="s">
         <v>50</v>
       </c>
@@ -3154,7 +3165,7 @@
       </c>
       <c r="M45" s="9"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A46" s="26" t="s">
         <v>51</v>
       </c>
@@ -3185,7 +3196,7 @@
       <c r="L46" s="8"/>
       <c r="M46" s="9"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A47" s="27" t="s">
         <v>52</v>
       </c>
@@ -3211,7 +3222,7 @@
       </c>
       <c r="M47" s="9"/>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A48" s="26" t="s">
         <v>53</v>
       </c>
@@ -3242,7 +3253,7 @@
       <c r="L48" s="8"/>
       <c r="M48" s="9"/>
     </row>
-    <row r="49" spans="1:229" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:229" x14ac:dyDescent="0.45">
       <c r="A49" s="27" t="s">
         <v>54</v>
       </c>
@@ -3268,7 +3279,7 @@
       </c>
       <c r="M49" s="9"/>
     </row>
-    <row r="50" spans="1:229" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:229" x14ac:dyDescent="0.45">
       <c r="A50" s="26" t="s">
         <v>55</v>
       </c>
@@ -3299,7 +3310,7 @@
       <c r="L50" s="8"/>
       <c r="M50" s="9"/>
     </row>
-    <row r="51" spans="1:229" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:229" x14ac:dyDescent="0.45">
       <c r="A51" s="27" t="s">
         <v>56</v>
       </c>
@@ -3328,7 +3339,7 @@
       </c>
       <c r="M51" s="9"/>
     </row>
-    <row r="52" spans="1:229" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:229" x14ac:dyDescent="0.45">
       <c r="A52" s="26" t="s">
         <v>59</v>
       </c>
@@ -3359,7 +3370,7 @@
       <c r="L52" s="8"/>
       <c r="M52" s="9"/>
     </row>
-    <row r="53" spans="1:229" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:229" x14ac:dyDescent="0.45">
       <c r="A53" s="27" t="s">
         <v>60</v>
       </c>
@@ -3385,7 +3396,7 @@
       </c>
       <c r="M53" s="9"/>
     </row>
-    <row r="54" spans="1:229" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:229" x14ac:dyDescent="0.45">
       <c r="A54" s="26" t="s">
         <v>61</v>
       </c>
@@ -3416,7 +3427,7 @@
       <c r="L54" s="8"/>
       <c r="M54" s="9"/>
     </row>
-    <row r="55" spans="1:229" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:229" x14ac:dyDescent="0.45">
       <c r="A55" s="27" t="s">
         <v>62</v>
       </c>
@@ -3442,7 +3453,7 @@
       </c>
       <c r="M55" s="9"/>
     </row>
-    <row r="56" spans="1:229" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:229" x14ac:dyDescent="0.45">
       <c r="A56" s="26" t="s">
         <v>63</v>
       </c>
@@ -3473,7 +3484,7 @@
       <c r="L56" s="8"/>
       <c r="M56" s="9"/>
     </row>
-    <row r="57" spans="1:229" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:229" x14ac:dyDescent="0.45">
       <c r="A57" s="27" t="s">
         <v>64</v>
       </c>
@@ -3499,7 +3510,7 @@
       </c>
       <c r="M57" s="9"/>
     </row>
-    <row r="58" spans="1:229" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:229" x14ac:dyDescent="0.45">
       <c r="A58" s="26" t="s">
         <v>65</v>
       </c>
@@ -3530,7 +3541,7 @@
       <c r="L58" s="8"/>
       <c r="M58" s="9"/>
     </row>
-    <row r="59" spans="1:229" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:229" x14ac:dyDescent="0.45">
       <c r="A59" s="27" t="s">
         <v>66</v>
       </c>
@@ -3559,7 +3570,7 @@
       </c>
       <c r="M59" s="9"/>
     </row>
-    <row r="60" spans="1:229" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:229" x14ac:dyDescent="0.45">
       <c r="A60" s="26" t="s">
         <v>68</v>
       </c>
@@ -3590,7 +3601,7 @@
       <c r="L60" s="8"/>
       <c r="M60" s="9"/>
     </row>
-    <row r="61" spans="1:229" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:229" x14ac:dyDescent="0.45">
       <c r="A61" s="27" t="s">
         <v>69</v>
       </c>
@@ -3616,7 +3627,7 @@
       </c>
       <c r="M61" s="9"/>
     </row>
-    <row r="62" spans="1:229" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:229" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A62" s="26" t="s">
         <v>70</v>
       </c>
@@ -3858,7 +3869,7 @@
       <c r="HT62" s="10"/>
       <c r="HU62" s="10"/>
     </row>
-    <row r="63" spans="1:229" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:229" x14ac:dyDescent="0.45">
       <c r="A63" s="27" t="s">
         <v>71</v>
       </c>
@@ -3884,7 +3895,7 @@
       </c>
       <c r="M63" s="9"/>
     </row>
-    <row r="64" spans="1:229" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:229" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A64" s="26" t="s">
         <v>72</v>
       </c>
@@ -4126,7 +4137,7 @@
       <c r="HT64" s="10"/>
       <c r="HU64" s="10"/>
     </row>
-    <row r="65" spans="1:229" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:229" x14ac:dyDescent="0.45">
       <c r="A65" s="27" t="s">
         <v>73</v>
       </c>
@@ -4152,7 +4163,7 @@
       </c>
       <c r="M65" s="9"/>
     </row>
-    <row r="66" spans="1:229" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:229" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A66" s="26" t="s">
         <v>74</v>
       </c>
@@ -4394,7 +4405,7 @@
       <c r="HT66" s="10"/>
       <c r="HU66" s="10"/>
     </row>
-    <row r="67" spans="1:229" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:229" x14ac:dyDescent="0.45">
       <c r="A67" s="27" t="s">
         <v>75</v>
       </c>
@@ -4420,7 +4431,7 @@
       </c>
       <c r="M67" s="9"/>
     </row>
-    <row r="68" spans="1:229" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:229" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A68" s="26" t="s">
         <v>76</v>
       </c>
@@ -4662,7 +4673,7 @@
       <c r="HT68" s="10"/>
       <c r="HU68" s="10"/>
     </row>
-    <row r="69" spans="1:229" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:229" x14ac:dyDescent="0.45">
       <c r="A69" s="27" t="s">
         <v>77</v>
       </c>
@@ -4688,7 +4699,7 @@
       </c>
       <c r="M69" s="9"/>
     </row>
-    <row r="70" spans="1:229" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:229" x14ac:dyDescent="0.45">
       <c r="A70" s="26" t="s">
         <v>78</v>
       </c>
@@ -4719,7 +4730,7 @@
       <c r="L70" s="8"/>
       <c r="M70" s="9"/>
     </row>
-    <row r="71" spans="1:229" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:229" x14ac:dyDescent="0.45">
       <c r="A71" s="27" t="s">
         <v>79</v>
       </c>
@@ -4750,7 +4761,7 @@
       <c r="Q71" s="13"/>
       <c r="R71" s="13"/>
     </row>
-    <row r="72" spans="1:229" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:229" x14ac:dyDescent="0.45">
       <c r="A72" s="26" t="s">
         <v>80</v>
       </c>
@@ -4778,12 +4789,12 @@
       <c r="I72" s="8"/>
       <c r="J72" s="8"/>
       <c r="K72" s="8"/>
-      <c r="L72" s="30"/>
+      <c r="L72" s="29"/>
       <c r="M72" s="12"/>
       <c r="N72" s="15"/>
       <c r="P72" s="16"/>
     </row>
-    <row r="73" spans="1:229" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:229" x14ac:dyDescent="0.45">
       <c r="A73" s="27" t="s">
         <v>81</v>
       </c>
@@ -4816,7 +4827,7 @@
       <c r="Q73" s="15"/>
       <c r="R73" s="15"/>
     </row>
-    <row r="74" spans="1:229" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:229" x14ac:dyDescent="0.45">
       <c r="A74" s="26" t="s">
         <v>83</v>
       </c>
@@ -4849,7 +4860,7 @@
       <c r="N74" s="15"/>
       <c r="O74" s="15"/>
     </row>
-    <row r="75" spans="1:229" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:229" x14ac:dyDescent="0.45">
       <c r="A75" s="27" t="s">
         <v>84</v>
       </c>
@@ -4875,7 +4886,7 @@
       </c>
       <c r="M75" s="9"/>
     </row>
-    <row r="76" spans="1:229" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:229" x14ac:dyDescent="0.45">
       <c r="A76" s="26" t="s">
         <v>85</v>
       </c>
@@ -4906,7 +4917,7 @@
       <c r="L76" s="8"/>
       <c r="M76" s="9"/>
     </row>
-    <row r="77" spans="1:229" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:229" x14ac:dyDescent="0.45">
       <c r="A77" s="27" t="s">
         <v>86</v>
       </c>
@@ -4932,7 +4943,7 @@
       </c>
       <c r="M77" s="9"/>
     </row>
-    <row r="78" spans="1:229" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:229" x14ac:dyDescent="0.45">
       <c r="A78" s="26" t="s">
         <v>87</v>
       </c>
@@ -4963,7 +4974,7 @@
       <c r="L78" s="8"/>
       <c r="M78" s="9"/>
     </row>
-    <row r="79" spans="1:229" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:229" x14ac:dyDescent="0.45">
       <c r="A79" s="27" t="s">
         <v>88</v>
       </c>
@@ -4989,7 +5000,7 @@
       </c>
       <c r="M79" s="9"/>
     </row>
-    <row r="80" spans="1:229" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:229" x14ac:dyDescent="0.45">
       <c r="A80" s="26" t="s">
         <v>89</v>
       </c>
@@ -5020,7 +5031,7 @@
       <c r="L80" s="8"/>
       <c r="M80" s="9"/>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A81" s="27" t="s">
         <v>90</v>
       </c>
@@ -5046,7 +5057,7 @@
       </c>
       <c r="M81" s="9"/>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A82" s="26" t="s">
         <v>91</v>
       </c>
@@ -5077,7 +5088,7 @@
       <c r="L82" s="8"/>
       <c r="M82" s="9"/>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A83" s="27" t="s">
         <v>92</v>
       </c>
@@ -5103,7 +5114,7 @@
       </c>
       <c r="M83" s="9"/>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A84" s="26" t="s">
         <v>93</v>
       </c>
@@ -5134,7 +5145,7 @@
       <c r="L84" s="8"/>
       <c r="M84" s="9"/>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A85" s="27" t="s">
         <v>94</v>
       </c>
@@ -5160,7 +5171,7 @@
       </c>
       <c r="M85" s="9"/>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A86" s="26" t="s">
         <v>95</v>
       </c>
@@ -5191,7 +5202,7 @@
       <c r="L86" s="8"/>
       <c r="M86" s="9"/>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A87" s="27" t="s">
         <v>96</v>
       </c>
@@ -5217,7 +5228,7 @@
       </c>
       <c r="M87" s="9"/>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A88" s="26" t="s">
         <v>97</v>
       </c>
@@ -5248,7 +5259,7 @@
       <c r="L88" s="8"/>
       <c r="M88" s="9"/>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A89" s="27" t="s">
         <v>98</v>
       </c>
@@ -5274,7 +5285,7 @@
       </c>
       <c r="M89" s="9"/>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A90" s="26" t="s">
         <v>99</v>
       </c>
@@ -5305,7 +5316,7 @@
       <c r="L90" s="8"/>
       <c r="M90" s="9"/>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A91" s="27" t="s">
         <v>100</v>
       </c>
@@ -5331,7 +5342,7 @@
       </c>
       <c r="M91" s="9"/>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A92" s="26" t="s">
         <v>101</v>
       </c>
@@ -5362,7 +5373,7 @@
       <c r="L92" s="8"/>
       <c r="M92" s="9"/>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A93" s="27" t="s">
         <v>102</v>
       </c>
@@ -5388,7 +5399,7 @@
       </c>
       <c r="M93" s="9"/>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A94" s="26" t="s">
         <v>103</v>
       </c>
@@ -5419,7 +5430,7 @@
       <c r="L94" s="8"/>
       <c r="M94" s="9"/>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A95" s="27" t="s">
         <v>104</v>
       </c>
@@ -5445,7 +5456,7 @@
       </c>
       <c r="M95" s="9"/>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A96" s="26" t="s">
         <v>105</v>
       </c>
@@ -5476,7 +5487,7 @@
       <c r="L96" s="8"/>
       <c r="M96" s="9"/>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A97" s="27" t="s">
         <v>106</v>
       </c>
@@ -5502,7 +5513,7 @@
       </c>
       <c r="M97" s="9"/>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A98" s="26" t="s">
         <v>107</v>
       </c>
@@ -5533,7 +5544,7 @@
       <c r="L98" s="8"/>
       <c r="M98" s="9"/>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A99" s="27" t="s">
         <v>108</v>
       </c>
@@ -5559,7 +5570,7 @@
       </c>
       <c r="M99" s="9"/>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A100" s="26" t="s">
         <v>109</v>
       </c>
@@ -5590,7 +5601,7 @@
       <c r="L100" s="8"/>
       <c r="M100" s="9"/>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A101" s="27" t="s">
         <v>110</v>
       </c>
@@ -5616,7 +5627,7 @@
       </c>
       <c r="M101" s="9"/>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A102" s="26" t="s">
         <v>111</v>
       </c>
@@ -5647,7 +5658,7 @@
       <c r="L102" s="8"/>
       <c r="M102" s="9"/>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A103" s="27" t="s">
         <v>112</v>
       </c>
@@ -5673,7 +5684,7 @@
       </c>
       <c r="M103" s="9"/>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A104" s="26" t="s">
         <v>113</v>
       </c>
@@ -5704,7 +5715,7 @@
       <c r="L104" s="8"/>
       <c r="M104" s="9"/>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A105" s="27" t="s">
         <v>114</v>
       </c>
@@ -5730,7 +5741,7 @@
       </c>
       <c r="M105" s="9"/>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A106" s="26" t="s">
         <v>115</v>
       </c>
@@ -5761,7 +5772,7 @@
       <c r="L106" s="8"/>
       <c r="M106" s="9"/>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A107" s="27" t="s">
         <v>116</v>
       </c>
@@ -5787,7 +5798,7 @@
       </c>
       <c r="M107" s="9"/>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A108" s="26" t="s">
         <v>117</v>
       </c>
@@ -5818,7 +5829,7 @@
       <c r="L108" s="8"/>
       <c r="M108" s="9"/>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A109" s="27" t="s">
         <v>118</v>
       </c>
@@ -5844,7 +5855,7 @@
       </c>
       <c r="M109" s="9"/>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A110" s="26" t="s">
         <v>119</v>
       </c>
@@ -5875,7 +5886,7 @@
       <c r="L110" s="8"/>
       <c r="M110" s="9"/>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A111" s="27" t="s">
         <v>120</v>
       </c>
@@ -5901,7 +5912,7 @@
       </c>
       <c r="M111" s="9"/>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A112" s="26" t="s">
         <v>121</v>
       </c>
@@ -5932,7 +5943,7 @@
       <c r="L112" s="8"/>
       <c r="M112" s="9"/>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A113" s="27" t="s">
         <v>122</v>
       </c>
@@ -5958,7 +5969,7 @@
       </c>
       <c r="M113" s="9"/>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A114" s="26" t="s">
         <v>123</v>
       </c>
@@ -5989,7 +6000,7 @@
       <c r="L114" s="8"/>
       <c r="M114" s="9"/>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A115" s="27" t="s">
         <v>124</v>
       </c>
@@ -6015,7 +6026,7 @@
       </c>
       <c r="M115" s="9"/>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A116" s="26" t="s">
         <v>125</v>
       </c>
@@ -6046,7 +6057,7 @@
       <c r="L116" s="8"/>
       <c r="M116" s="9"/>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A117" s="27" t="s">
         <v>126</v>
       </c>
@@ -6072,7 +6083,7 @@
       </c>
       <c r="M117" s="9"/>
     </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A118" s="26" t="s">
         <v>127</v>
       </c>
@@ -6103,7 +6114,7 @@
       <c r="L118" s="8"/>
       <c r="M118" s="9"/>
     </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A119" s="27" t="s">
         <v>128</v>
       </c>
@@ -6129,7 +6140,7 @@
       </c>
       <c r="M119" s="9"/>
     </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A120" s="26" t="s">
         <v>129</v>
       </c>
@@ -6160,7 +6171,7 @@
       <c r="L120" s="8"/>
       <c r="M120" s="9"/>
     </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A121" s="27" t="s">
         <v>130</v>
       </c>
@@ -6186,7 +6197,7 @@
       </c>
       <c r="M121" s="9"/>
     </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A122" s="26" t="s">
         <v>131</v>
       </c>
@@ -6217,7 +6228,7 @@
       <c r="L122" s="8"/>
       <c r="M122" s="9"/>
     </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A123" s="27" t="s">
         <v>132</v>
       </c>
@@ -6243,7 +6254,7 @@
       </c>
       <c r="M123" s="9"/>
     </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A124" s="26" t="s">
         <v>133</v>
       </c>
@@ -6274,7 +6285,7 @@
       <c r="L124" s="8"/>
       <c r="M124" s="9"/>
     </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A125" s="27" t="s">
         <v>134</v>
       </c>
@@ -6300,7 +6311,7 @@
       </c>
       <c r="M125" s="9"/>
     </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A126" s="26" t="s">
         <v>135</v>
       </c>
@@ -6331,7 +6342,7 @@
       <c r="L126" s="8"/>
       <c r="M126" s="9"/>
     </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A127" s="27" t="s">
         <v>136</v>
       </c>
@@ -6357,7 +6368,7 @@
       </c>
       <c r="M127" s="9"/>
     </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A128" s="26" t="s">
         <v>137</v>
       </c>
@@ -6388,7 +6399,7 @@
       <c r="L128" s="8"/>
       <c r="M128" s="9"/>
     </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A129" s="27" t="s">
         <v>138</v>
       </c>
@@ -6414,7 +6425,7 @@
       </c>
       <c r="M129" s="9"/>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A130" s="26" t="s">
         <v>139</v>
       </c>
@@ -6445,7 +6456,7 @@
       <c r="L130" s="8"/>
       <c r="M130" s="9"/>
     </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A131" s="27" t="s">
         <v>140</v>
       </c>
@@ -6471,7 +6482,7 @@
       </c>
       <c r="M131" s="9"/>
     </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A132" s="26" t="s">
         <v>141</v>
       </c>
@@ -6502,7 +6513,7 @@
       <c r="L132" s="8"/>
       <c r="M132" s="9"/>
     </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A133" s="27" t="s">
         <v>142</v>
       </c>
@@ -6528,7 +6539,7 @@
       </c>
       <c r="M133" s="9"/>
     </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A134" s="26" t="s">
         <v>143</v>
       </c>
@@ -6559,7 +6570,7 @@
       <c r="L134" s="8"/>
       <c r="M134" s="9"/>
     </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A135" s="27" t="s">
         <v>144</v>
       </c>
@@ -6585,7 +6596,7 @@
       </c>
       <c r="M135" s="9"/>
     </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A136" s="26" t="s">
         <v>145</v>
       </c>
@@ -6616,7 +6627,7 @@
       <c r="L136" s="8"/>
       <c r="M136" s="9"/>
     </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A137" s="27" t="s">
         <v>146</v>
       </c>
@@ -6642,7 +6653,7 @@
       </c>
       <c r="M137" s="9"/>
     </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A138" s="26" t="s">
         <v>147</v>
       </c>
@@ -6673,7 +6684,7 @@
       <c r="L138" s="8"/>
       <c r="M138" s="9"/>
     </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A139" s="27" t="s">
         <v>148</v>
       </c>
@@ -6699,7 +6710,7 @@
       </c>
       <c r="M139" s="9"/>
     </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A140" s="26" t="s">
         <v>149</v>
       </c>
@@ -6730,7 +6741,7 @@
       <c r="L140" s="8"/>
       <c r="M140" s="9"/>
     </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A141" s="27" t="s">
         <v>150</v>
       </c>
@@ -6756,7 +6767,7 @@
       </c>
       <c r="M141" s="9"/>
     </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A142" s="26" t="s">
         <v>151</v>
       </c>
@@ -6787,7 +6798,7 @@
       <c r="L142" s="8"/>
       <c r="M142" s="9"/>
     </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A143" s="27" t="s">
         <v>152</v>
       </c>
@@ -6813,7 +6824,7 @@
       </c>
       <c r="M143" s="9"/>
     </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A144" s="26" t="s">
         <v>153</v>
       </c>
@@ -6844,7 +6855,7 @@
       <c r="L144" s="8"/>
       <c r="M144" s="9"/>
     </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A145" s="27" t="s">
         <v>154</v>
       </c>
@@ -6870,7 +6881,7 @@
       </c>
       <c r="M145" s="9"/>
     </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A146" s="26" t="s">
         <v>155</v>
       </c>
@@ -6901,7 +6912,7 @@
       <c r="L146" s="8"/>
       <c r="M146" s="9"/>
     </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A147" s="27" t="s">
         <v>156</v>
       </c>
@@ -6927,7 +6938,7 @@
       </c>
       <c r="M147" s="9"/>
     </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A148" s="26" t="s">
         <v>157</v>
       </c>
@@ -6958,7 +6969,7 @@
       <c r="L148" s="8"/>
       <c r="M148" s="9"/>
     </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A149" s="27" t="s">
         <v>158</v>
       </c>
@@ -6984,7 +6995,7 @@
       </c>
       <c r="M149" s="9"/>
     </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A150" s="26" t="s">
         <v>159</v>
       </c>
@@ -7015,7 +7026,7 @@
       <c r="L150" s="8"/>
       <c r="M150" s="9"/>
     </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A151" s="27" t="s">
         <v>160</v>
       </c>
@@ -7041,7 +7052,7 @@
       </c>
       <c r="M151" s="9"/>
     </row>
-    <row r="152" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A152" s="26" t="s">
         <v>161</v>
       </c>
@@ -7072,7 +7083,7 @@
       <c r="L152" s="8"/>
       <c r="M152" s="9"/>
     </row>
-    <row r="153" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A153" s="27" t="s">
         <v>162</v>
       </c>
@@ -7098,7 +7109,7 @@
       </c>
       <c r="M153" s="9"/>
     </row>
-    <row r="154" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A154" s="26" t="s">
         <v>163</v>
       </c>
@@ -7129,7 +7140,7 @@
       <c r="L154" s="8"/>
       <c r="M154" s="9"/>
     </row>
-    <row r="155" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A155" s="27" t="s">
         <v>164</v>
       </c>
@@ -7155,7 +7166,7 @@
       </c>
       <c r="M155" s="9"/>
     </row>
-    <row r="156" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A156" s="26" t="s">
         <v>165</v>
       </c>
@@ -7186,7 +7197,7 @@
       <c r="L156" s="8"/>
       <c r="M156" s="9"/>
     </row>
-    <row r="157" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A157" s="27" t="s">
         <v>166</v>
       </c>
@@ -7212,7 +7223,7 @@
       </c>
       <c r="M157" s="9"/>
     </row>
-    <row r="158" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A158" s="26" t="s">
         <v>167</v>
       </c>
@@ -7251,7 +7262,7 @@
       <c r="L158" s="8"/>
       <c r="M158" s="9"/>
     </row>
-    <row r="159" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A159" s="27" t="s">
         <v>169</v>
       </c>
@@ -7277,7 +7288,7 @@
       </c>
       <c r="M159" s="9"/>
     </row>
-    <row r="160" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A160" s="26" t="s">
         <v>170</v>
       </c>
@@ -7316,7 +7327,7 @@
       <c r="L160" s="8"/>
       <c r="M160" s="9"/>
     </row>
-    <row r="161" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A161" s="27" t="s">
         <v>171</v>
       </c>
@@ -7342,7 +7353,7 @@
       </c>
       <c r="M161" s="9"/>
     </row>
-    <row r="162" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A162" s="26" t="s">
         <v>172</v>
       </c>
@@ -7373,7 +7384,7 @@
       <c r="L162" s="8"/>
       <c r="M162" s="9"/>
     </row>
-    <row r="163" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A163" s="27" t="s">
         <v>173</v>
       </c>
@@ -7399,7 +7410,7 @@
       </c>
       <c r="M163" s="9"/>
     </row>
-    <row r="164" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A164" s="26" t="s">
         <v>174</v>
       </c>
@@ -7430,7 +7441,7 @@
       <c r="L164" s="8"/>
       <c r="M164" s="9"/>
     </row>
-    <row r="165" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A165" s="27" t="s">
         <v>175</v>
       </c>
@@ -7468,7 +7479,7 @@
       </c>
       <c r="M165" s="9"/>
     </row>
-    <row r="166" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A166" s="26" t="s">
         <v>176</v>
       </c>
@@ -7499,7 +7510,7 @@
       <c r="L166" s="8"/>
       <c r="M166" s="9"/>
     </row>
-    <row r="167" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A167" s="27" t="s">
         <v>177</v>
       </c>
@@ -7525,7 +7536,7 @@
       </c>
       <c r="M167" s="9"/>
     </row>
-    <row r="168" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A168" s="26" t="s">
         <v>178</v>
       </c>
@@ -7556,7 +7567,7 @@
       <c r="L168" s="8"/>
       <c r="M168" s="9"/>
     </row>
-    <row r="169" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A169" s="27" t="s">
         <v>179</v>
       </c>
@@ -7582,7 +7593,7 @@
       </c>
       <c r="M169" s="9"/>
     </row>
-    <row r="170" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A170" s="26" t="s">
         <v>180</v>
       </c>
@@ -7613,7 +7624,7 @@
       <c r="L170" s="8"/>
       <c r="M170" s="9"/>
     </row>
-    <row r="171" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A171" s="27" t="s">
         <v>181</v>
       </c>
@@ -7639,7 +7650,7 @@
       </c>
       <c r="M171" s="9"/>
     </row>
-    <row r="172" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A172" s="26" t="s">
         <v>182</v>
       </c>
@@ -7670,7 +7681,7 @@
       <c r="L172" s="8"/>
       <c r="M172" s="9"/>
     </row>
-    <row r="173" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A173" s="27" t="s">
         <v>183</v>
       </c>
@@ -7696,7 +7707,7 @@
       </c>
       <c r="M173" s="9"/>
     </row>
-    <row r="174" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A174" s="26" t="s">
         <v>184</v>
       </c>
@@ -7727,7 +7738,7 @@
       <c r="L174" s="8"/>
       <c r="M174" s="9"/>
     </row>
-    <row r="175" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A175" s="27" t="s">
         <v>185</v>
       </c>
@@ -7753,7 +7764,7 @@
       </c>
       <c r="M175" s="9"/>
     </row>
-    <row r="176" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A176" s="26" t="s">
         <v>186</v>
       </c>
@@ -7792,7 +7803,7 @@
       <c r="L176" s="8"/>
       <c r="M176" s="9"/>
     </row>
-    <row r="177" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A177" s="27" t="s">
         <v>187</v>
       </c>
@@ -7818,7 +7829,7 @@
       </c>
       <c r="M177" s="9"/>
     </row>
-    <row r="178" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A178" s="26" t="s">
         <v>188</v>
       </c>
@@ -7849,7 +7860,7 @@
       <c r="L178" s="8"/>
       <c r="M178" s="9"/>
     </row>
-    <row r="179" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A179" s="27" t="s">
         <v>189</v>
       </c>
@@ -7875,7 +7886,7 @@
       </c>
       <c r="M179" s="9"/>
     </row>
-    <row r="180" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A180" s="26" t="s">
         <v>190</v>
       </c>
@@ -7906,7 +7917,7 @@
       <c r="L180" s="8"/>
       <c r="M180" s="9"/>
     </row>
-    <row r="181" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A181" s="27" t="s">
         <v>191</v>
       </c>
@@ -7932,7 +7943,7 @@
       </c>
       <c r="M181" s="9"/>
     </row>
-    <row r="182" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A182" s="26" t="s">
         <v>192</v>
       </c>
@@ -7963,7 +7974,7 @@
       <c r="L182" s="8"/>
       <c r="M182" s="9"/>
     </row>
-    <row r="183" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A183" s="27" t="s">
         <v>193</v>
       </c>
@@ -7989,7 +8000,7 @@
       </c>
       <c r="M183" s="9"/>
     </row>
-    <row r="184" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A184" s="26" t="s">
         <v>194</v>
       </c>
@@ -8020,7 +8031,7 @@
       <c r="L184" s="8"/>
       <c r="M184" s="9"/>
     </row>
-    <row r="185" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A185" s="27" t="s">
         <v>195</v>
       </c>
@@ -8046,7 +8057,7 @@
       </c>
       <c r="M185" s="9"/>
     </row>
-    <row r="186" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A186" s="26" t="s">
         <v>196</v>
       </c>
@@ -8077,7 +8088,7 @@
       <c r="L186" s="8"/>
       <c r="M186" s="9"/>
     </row>
-    <row r="187" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A187" s="27" t="s">
         <v>197</v>
       </c>
@@ -8103,7 +8114,7 @@
       </c>
       <c r="M187" s="9"/>
     </row>
-    <row r="188" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A188" s="26" t="s">
         <v>198</v>
       </c>
@@ -8134,7 +8145,7 @@
       <c r="L188" s="8"/>
       <c r="M188" s="9"/>
     </row>
-    <row r="189" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A189" s="27" t="s">
         <v>199</v>
       </c>
@@ -8172,7 +8183,7 @@
       </c>
       <c r="M189" s="9"/>
     </row>
-    <row r="190" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A190" s="26" t="s">
         <v>200</v>
       </c>
@@ -8209,7 +8220,7 @@
       <c r="L190" s="8"/>
       <c r="M190" s="9"/>
     </row>
-    <row r="191" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A191" s="27" t="s">
         <v>201</v>
       </c>
@@ -8235,7 +8246,7 @@
       </c>
       <c r="M191" s="9"/>
     </row>
-    <row r="192" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A192" s="26" t="s">
         <v>202</v>
       </c>
@@ -8274,7 +8285,7 @@
       <c r="L192" s="8"/>
       <c r="M192" s="9"/>
     </row>
-    <row r="193" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A193" s="27" t="s">
         <v>203</v>
       </c>
@@ -8300,7 +8311,7 @@
       </c>
       <c r="M193" s="9"/>
     </row>
-    <row r="194" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A194" s="26" t="s">
         <v>204</v>
       </c>
@@ -8331,7 +8342,7 @@
       <c r="L194" s="8"/>
       <c r="M194" s="9"/>
     </row>
-    <row r="195" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A195" s="27" t="s">
         <v>205</v>
       </c>
@@ -8357,7 +8368,7 @@
       </c>
       <c r="M195" s="9"/>
     </row>
-    <row r="196" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A196" s="26" t="s">
         <v>206</v>
       </c>
@@ -8388,7 +8399,7 @@
       <c r="L196" s="8"/>
       <c r="M196" s="9"/>
     </row>
-    <row r="197" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A197" s="27" t="s">
         <v>207</v>
       </c>
@@ -8414,7 +8425,7 @@
       </c>
       <c r="M197" s="9"/>
     </row>
-    <row r="198" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A198" s="26" t="s">
         <v>208</v>
       </c>
@@ -8445,7 +8456,7 @@
       <c r="L198" s="8"/>
       <c r="M198" s="9"/>
     </row>
-    <row r="199" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A199" s="27" t="s">
         <v>209</v>
       </c>
@@ -8471,7 +8482,7 @@
       </c>
       <c r="M199" s="9"/>
     </row>
-    <row r="200" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A200" s="26" t="s">
         <v>210</v>
       </c>
@@ -8502,7 +8513,7 @@
       <c r="L200" s="8"/>
       <c r="M200" s="9"/>
     </row>
-    <row r="201" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A201" s="27" t="s">
         <v>211</v>
       </c>
@@ -8528,7 +8539,7 @@
       </c>
       <c r="M201" s="9"/>
     </row>
-    <row r="202" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A202" s="26" t="s">
         <v>212</v>
       </c>
@@ -8559,7 +8570,7 @@
       <c r="L202" s="8"/>
       <c r="M202" s="9"/>
     </row>
-    <row r="203" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A203" s="27" t="s">
         <v>213</v>
       </c>
@@ -8585,7 +8596,7 @@
       </c>
       <c r="M203" s="9"/>
     </row>
-    <row r="204" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A204" s="26" t="s">
         <v>214</v>
       </c>
@@ -8616,7 +8627,7 @@
       <c r="L204" s="8"/>
       <c r="M204" s="9"/>
     </row>
-    <row r="205" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A205" s="27" t="s">
         <v>215</v>
       </c>
@@ -8642,7 +8653,7 @@
       </c>
       <c r="M205" s="9"/>
     </row>
-    <row r="206" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A206" s="26" t="s">
         <v>216</v>
       </c>
@@ -8673,7 +8684,7 @@
       <c r="L206" s="8"/>
       <c r="M206" s="9"/>
     </row>
-    <row r="207" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A207" s="27" t="s">
         <v>217</v>
       </c>
@@ -8699,7 +8710,7 @@
       </c>
       <c r="M207" s="9"/>
     </row>
-    <row r="208" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A208" s="26" t="s">
         <v>218</v>
       </c>
@@ -8730,7 +8741,7 @@
       <c r="L208" s="8"/>
       <c r="M208" s="9"/>
     </row>
-    <row r="209" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A209" s="27" t="s">
         <v>219</v>
       </c>
@@ -8756,7 +8767,7 @@
       </c>
       <c r="M209" s="9"/>
     </row>
-    <row r="210" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A210" s="26" t="s">
         <v>220</v>
       </c>
@@ -8787,7 +8798,7 @@
       <c r="L210" s="8"/>
       <c r="M210" s="9"/>
     </row>
-    <row r="211" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A211" s="27" t="s">
         <v>221</v>
       </c>
@@ -8813,7 +8824,7 @@
       </c>
       <c r="M211" s="9"/>
     </row>
-    <row r="212" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A212" s="26" t="s">
         <v>222</v>
       </c>
@@ -8844,7 +8855,7 @@
       <c r="L212" s="8"/>
       <c r="M212" s="9"/>
     </row>
-    <row r="213" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A213" s="27" t="s">
         <v>223</v>
       </c>
@@ -8870,7 +8881,7 @@
       </c>
       <c r="M213" s="9"/>
     </row>
-    <row r="214" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A214" s="26" t="s">
         <v>224</v>
       </c>
@@ -8901,7 +8912,7 @@
       <c r="L214" s="8"/>
       <c r="M214" s="9"/>
     </row>
-    <row r="215" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A215" s="27" t="s">
         <v>225</v>
       </c>
@@ -8927,7 +8938,7 @@
       </c>
       <c r="M215" s="9"/>
     </row>
-    <row r="216" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A216" s="26" t="s">
         <v>226</v>
       </c>
@@ -8958,7 +8969,7 @@
       <c r="L216" s="8"/>
       <c r="M216" s="9"/>
     </row>
-    <row r="217" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A217" s="27" t="s">
         <v>227</v>
       </c>
@@ -8984,7 +8995,7 @@
       </c>
       <c r="M217" s="9"/>
     </row>
-    <row r="218" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A218" s="26" t="s">
         <v>228</v>
       </c>
@@ -9023,7 +9034,7 @@
       <c r="L218" s="8"/>
       <c r="M218" s="9"/>
     </row>
-    <row r="219" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A219" s="27" t="s">
         <v>229</v>
       </c>
@@ -9049,7 +9060,7 @@
       </c>
       <c r="M219" s="9"/>
     </row>
-    <row r="220" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A220" s="26" t="s">
         <v>230</v>
       </c>
@@ -9080,7 +9091,7 @@
       <c r="L220" s="8"/>
       <c r="M220" s="9"/>
     </row>
-    <row r="221" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A221" s="27" t="s">
         <v>231</v>
       </c>
@@ -9106,7 +9117,7 @@
       </c>
       <c r="M221" s="9"/>
     </row>
-    <row r="222" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A222" s="26" t="s">
         <v>232</v>
       </c>
@@ -9137,7 +9148,7 @@
       <c r="L222" s="8"/>
       <c r="M222" s="9"/>
     </row>
-    <row r="223" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A223" s="27" t="s">
         <v>233</v>
       </c>
@@ -9163,7 +9174,7 @@
       </c>
       <c r="M223" s="9"/>
     </row>
-    <row r="224" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A224" s="26" t="s">
         <v>234</v>
       </c>
@@ -9194,7 +9205,7 @@
       <c r="L224" s="8"/>
       <c r="M224" s="9"/>
     </row>
-    <row r="225" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A225" s="27" t="s">
         <v>235</v>
       </c>
@@ -9220,7 +9231,7 @@
       </c>
       <c r="M225" s="9"/>
     </row>
-    <row r="226" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A226" s="26" t="s">
         <v>236</v>
       </c>
@@ -9251,7 +9262,7 @@
       <c r="L226" s="8"/>
       <c r="M226" s="9"/>
     </row>
-    <row r="227" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A227" s="27" t="s">
         <v>237</v>
       </c>
@@ -9277,7 +9288,7 @@
       </c>
       <c r="M227" s="9"/>
     </row>
-    <row r="228" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A228" s="26" t="s">
         <v>238</v>
       </c>
@@ -9308,7 +9319,7 @@
       <c r="L228" s="8"/>
       <c r="M228" s="9"/>
     </row>
-    <row r="229" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A229" s="27" t="s">
         <v>239</v>
       </c>
@@ -9334,7 +9345,7 @@
       </c>
       <c r="M229" s="9"/>
     </row>
-    <row r="230" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A230" s="26" t="s">
         <v>240</v>
       </c>
@@ -9365,7 +9376,7 @@
       <c r="L230" s="8"/>
       <c r="M230" s="9"/>
     </row>
-    <row r="231" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A231" s="27" t="s">
         <v>241</v>
       </c>
@@ -9391,7 +9402,7 @@
       </c>
       <c r="M231" s="9"/>
     </row>
-    <row r="232" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A232" s="26" t="s">
         <v>242</v>
       </c>
@@ -9422,7 +9433,7 @@
       <c r="L232" s="8"/>
       <c r="M232" s="9"/>
     </row>
-    <row r="233" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A233" s="27" t="s">
         <v>243</v>
       </c>
@@ -9448,7 +9459,7 @@
       </c>
       <c r="M233" s="9"/>
     </row>
-    <row r="234" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A234" s="26" t="s">
         <v>244</v>
       </c>
@@ -9479,7 +9490,7 @@
       <c r="L234" s="8"/>
       <c r="M234" s="9"/>
     </row>
-    <row r="235" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A235" s="27" t="s">
         <v>245</v>
       </c>
@@ -9517,7 +9528,7 @@
       </c>
       <c r="M235" s="9"/>
     </row>
-    <row r="236" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A236" s="26" t="s">
         <v>246</v>
       </c>
@@ -9556,7 +9567,7 @@
       <c r="L236" s="8"/>
       <c r="M236" s="9"/>
     </row>
-    <row r="237" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A237" s="27" t="s">
         <v>247</v>
       </c>
@@ -9582,7 +9593,7 @@
       </c>
       <c r="M237" s="9"/>
     </row>
-    <row r="238" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A238" s="26" t="s">
         <v>248</v>
       </c>
@@ -9613,7 +9624,7 @@
       <c r="L238" s="8"/>
       <c r="M238" s="9"/>
     </row>
-    <row r="239" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A239" s="27" t="s">
         <v>249</v>
       </c>
@@ -9639,7 +9650,7 @@
       </c>
       <c r="M239" s="9"/>
     </row>
-    <row r="240" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A240" s="26" t="s">
         <v>250</v>
       </c>
@@ -9670,7 +9681,7 @@
       <c r="L240" s="8"/>
       <c r="M240" s="9"/>
     </row>
-    <row r="241" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A241" s="27" t="s">
         <v>251</v>
       </c>
@@ -9696,7 +9707,7 @@
       </c>
       <c r="M241" s="9"/>
     </row>
-    <row r="242" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A242" s="26" t="s">
         <v>252</v>
       </c>
@@ -9727,7 +9738,7 @@
       <c r="L242" s="8"/>
       <c r="M242" s="9"/>
     </row>
-    <row r="243" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A243" s="27" t="s">
         <v>253</v>
       </c>
@@ -9753,7 +9764,7 @@
       </c>
       <c r="M243" s="9"/>
     </row>
-    <row r="244" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A244" s="26" t="s">
         <v>254</v>
       </c>
@@ -9792,7 +9803,7 @@
       <c r="L244" s="8"/>
       <c r="M244" s="9"/>
     </row>
-    <row r="245" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A245" s="27" t="s">
         <v>255</v>
       </c>
@@ -9818,7 +9829,7 @@
       </c>
       <c r="M245" s="9"/>
     </row>
-    <row r="246" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A246" s="26" t="s">
         <v>256</v>
       </c>
@@ -9849,7 +9860,7 @@
       <c r="L246" s="8"/>
       <c r="M246" s="9"/>
     </row>
-    <row r="247" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A247" s="27" t="s">
         <v>257</v>
       </c>
@@ -9887,7 +9898,7 @@
       </c>
       <c r="M247" s="9"/>
     </row>
-    <row r="248" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A248" s="26" t="s">
         <v>258</v>
       </c>
@@ -9918,7 +9929,7 @@
       <c r="L248" s="8"/>
       <c r="M248" s="9"/>
     </row>
-    <row r="249" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A249" s="27" t="s">
         <v>259</v>
       </c>
@@ -9944,7 +9955,7 @@
       </c>
       <c r="M249" s="9"/>
     </row>
-    <row r="250" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A250" s="26" t="s">
         <v>260</v>
       </c>
@@ -9975,7 +9986,7 @@
       <c r="L250" s="8"/>
       <c r="M250" s="9"/>
     </row>
-    <row r="251" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A251" s="27" t="s">
         <v>261</v>
       </c>
@@ -10001,7 +10012,7 @@
       </c>
       <c r="M251" s="9"/>
     </row>
-    <row r="252" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A252" s="26" t="s">
         <v>262</v>
       </c>
@@ -10032,7 +10043,7 @@
       <c r="L252" s="8"/>
       <c r="M252" s="9"/>
     </row>
-    <row r="253" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A253" s="27" t="s">
         <v>263</v>
       </c>
@@ -10058,7 +10069,7 @@
       </c>
       <c r="M253" s="9"/>
     </row>
-    <row r="254" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A254" s="26" t="s">
         <v>264</v>
       </c>
@@ -10089,7 +10100,7 @@
       <c r="L254" s="8"/>
       <c r="M254" s="9"/>
     </row>
-    <row r="255" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A255" s="27" t="s">
         <v>265</v>
       </c>
@@ -10115,7 +10126,7 @@
       </c>
       <c r="M255" s="9"/>
     </row>
-    <row r="256" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A256" s="26" t="s">
         <v>266</v>
       </c>
@@ -10146,7 +10157,7 @@
       <c r="L256" s="8"/>
       <c r="M256" s="9"/>
     </row>
-    <row r="257" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A257" s="27" t="s">
         <v>267</v>
       </c>
@@ -10172,7 +10183,7 @@
       </c>
       <c r="M257" s="9"/>
     </row>
-    <row r="258" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A258" s="26" t="s">
         <v>268</v>
       </c>
@@ -10203,7 +10214,7 @@
       <c r="L258" s="8"/>
       <c r="M258" s="9"/>
     </row>
-    <row r="259" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A259" s="27" t="s">
         <v>269</v>
       </c>
@@ -10229,7 +10240,7 @@
       </c>
       <c r="M259" s="9"/>
     </row>
-    <row r="260" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A260" s="26" t="s">
         <v>270</v>
       </c>
@@ -10260,7 +10271,7 @@
       <c r="L260" s="8"/>
       <c r="M260" s="9"/>
     </row>
-    <row r="261" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A261" s="27" t="s">
         <v>271</v>
       </c>
@@ -10286,7 +10297,7 @@
       </c>
       <c r="M261" s="9"/>
     </row>
-    <row r="262" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A262" s="26" t="s">
         <v>272</v>
       </c>
@@ -10317,7 +10328,7 @@
       <c r="L262" s="8"/>
       <c r="M262" s="9"/>
     </row>
-    <row r="263" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A263" s="27" t="s">
         <v>273</v>
       </c>
@@ -10343,7 +10354,7 @@
       </c>
       <c r="M263" s="9"/>
     </row>
-    <row r="264" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A264" s="26" t="s">
         <v>274</v>
       </c>
@@ -10374,7 +10385,7 @@
       <c r="L264" s="8"/>
       <c r="M264" s="9"/>
     </row>
-    <row r="265" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A265" s="27" t="s">
         <v>275</v>
       </c>
@@ -10403,7 +10414,7 @@
       </c>
       <c r="M265" s="9"/>
     </row>
-    <row r="266" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A266" s="26" t="s">
         <v>276</v>
       </c>
@@ -10442,7 +10453,7 @@
       <c r="L266" s="8"/>
       <c r="M266" s="9"/>
     </row>
-    <row r="267" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A267" s="27" t="s">
         <v>277</v>
       </c>
@@ -10468,7 +10479,7 @@
       </c>
       <c r="M267" s="9"/>
     </row>
-    <row r="268" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A268" s="26" t="s">
         <v>278</v>
       </c>
@@ -10499,7 +10510,7 @@
       <c r="L268" s="8"/>
       <c r="M268" s="9"/>
     </row>
-    <row r="269" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A269" s="27" t="s">
         <v>279</v>
       </c>
@@ -10528,7 +10539,7 @@
       </c>
       <c r="M269" s="9"/>
     </row>
-    <row r="270" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A270" s="9"/>
       <c r="B270" s="9"/>
       <c r="C270" s="9"/>
@@ -10543,7 +10554,7 @@
       <c r="L270" s="9"/>
       <c r="M270" s="9"/>
     </row>
-    <row r="272" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A272" s="18" t="s">
         <v>280</v>
       </c>
@@ -10551,7 +10562,7 @@
         <v>1882</v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A273" s="19" t="s">
         <v>281</v>
       </c>
@@ -10559,11 +10570,11 @@
         <v>1867</v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A274" s="28" t="s">
         <v>390</v>
       </c>
-      <c r="E274" s="29">
+      <c r="E274" s="28">
         <v>545</v>
       </c>
     </row>
@@ -10576,33 +10587,33 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:HV116"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M88" sqref="M88"/>
+      <selection pane="bottomLeft" activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="15" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="31.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24" style="10" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" style="10" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" style="10" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="24.85546875" style="10" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="21.140625" style="10" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="20.85546875" style="10" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="31.53515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24" style="10" customWidth="1"/>
+    <col min="3" max="3" width="20.69140625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="13.84375" style="10" customWidth="1"/>
+    <col min="5" max="5" width="24.84375" style="10" customWidth="1"/>
+    <col min="6" max="6" width="21.15234375" style="10" customWidth="1"/>
+    <col min="7" max="7" width="20.84375" style="10" customWidth="1"/>
     <col min="8" max="8" width="10" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="49.42578125" style="10" customWidth="1"/>
+    <col min="9" max="9" width="10.84375" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.53515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.53515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="49.3828125" style="10" customWidth="1"/>
     <col min="14" max="14" width="1" style="10" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="10"/>
+    <col min="15" max="16384" width="9.15234375" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -10627,22 +10638,22 @@
       <c r="W1" s="21"/>
       <c r="X1" s="22"/>
     </row>
-    <row r="2" spans="1:24" s="2" customFormat="1" ht="61.5" x14ac:dyDescent="0.85">
-      <c r="A2" s="31" t="s">
+    <row r="2" spans="1:24" s="2" customFormat="1" ht="61.75" x14ac:dyDescent="1.5">
+      <c r="A2" s="30" t="s">
         <v>395</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
       <c r="N2" s="23"/>
       <c r="O2" s="23"/>
       <c r="P2" s="23"/>
@@ -10655,7 +10666,7 @@
       <c r="W2" s="23"/>
       <c r="X2" s="24"/>
     </row>
-    <row r="3" spans="1:24" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="1.05">
+    <row r="3" spans="1:24" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="1.75">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -10670,7 +10681,7 @@
       <c r="L3" s="4"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:24" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -10685,7 +10696,7 @@
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="1:24" s="7" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" s="7" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
@@ -10727,7 +10738,7 @@
       </c>
       <c r="N5" s="6"/>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A6" s="26" t="s">
         <v>381</v>
       </c>
@@ -10767,7 +10778,7 @@
       <c r="M6" s="8"/>
       <c r="N6" s="9"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A7" s="27" t="s">
         <v>358</v>
       </c>
@@ -10806,7 +10817,7 @@
       </c>
       <c r="N7" s="9"/>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A8" s="26" t="s">
         <v>310</v>
       </c>
@@ -10847,7 +10858,7 @@
       <c r="M8" s="8"/>
       <c r="N8" s="9"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A9" s="27" t="s">
         <v>312</v>
       </c>
@@ -10887,7 +10898,7 @@
       </c>
       <c r="N9" s="9"/>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A10" s="26" t="s">
         <v>282</v>
       </c>
@@ -10929,7 +10940,7 @@
       <c r="M10" s="8"/>
       <c r="N10" s="9"/>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A11" s="27" t="s">
         <v>386</v>
       </c>
@@ -10968,7 +10979,7 @@
       </c>
       <c r="N11" s="9"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A12" s="26" t="s">
         <v>313</v>
       </c>
@@ -11009,7 +11020,7 @@
       <c r="M12" s="8"/>
       <c r="N12" s="9"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A13" s="27" t="s">
         <v>388</v>
       </c>
@@ -11048,7 +11059,7 @@
       </c>
       <c r="N13" s="9"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A14" s="26" t="s">
         <v>363</v>
       </c>
@@ -11090,7 +11101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A15" s="27" t="s">
         <v>366</v>
       </c>
@@ -11129,7 +11140,7 @@
       </c>
       <c r="N15" s="9"/>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A16" s="26" t="s">
         <v>311</v>
       </c>
@@ -11170,7 +11181,7 @@
       <c r="M16" s="8"/>
       <c r="N16" s="9"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A17" s="27" t="s">
         <v>285</v>
       </c>
@@ -11211,7 +11222,7 @@
       </c>
       <c r="N17" s="9"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A18" s="26" t="s">
         <v>317</v>
       </c>
@@ -11252,7 +11263,7 @@
       <c r="M18" s="8"/>
       <c r="N18" s="9"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A19" s="27" t="s">
         <v>359</v>
       </c>
@@ -11291,7 +11302,7 @@
       </c>
       <c r="N19" s="9"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A20" s="26" t="s">
         <v>286</v>
       </c>
@@ -11333,7 +11344,7 @@
       <c r="M20" s="8"/>
       <c r="N20" s="9"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A21" s="27" t="s">
         <v>318</v>
       </c>
@@ -11373,7 +11384,7 @@
       </c>
       <c r="N21" s="9"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A22" s="26" t="s">
         <v>352</v>
       </c>
@@ -11413,7 +11424,7 @@
       <c r="M22" s="8"/>
       <c r="N22" s="9"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A23" s="27" t="s">
         <v>377</v>
       </c>
@@ -11452,7 +11463,7 @@
       </c>
       <c r="N23" s="9"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A24" s="26" t="s">
         <v>356</v>
       </c>
@@ -11492,7 +11503,7 @@
       <c r="M24" s="8"/>
       <c r="N24" s="9"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A25" s="27" t="s">
         <v>319</v>
       </c>
@@ -11532,7 +11543,7 @@
       </c>
       <c r="N25" s="9"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A26" s="26" t="s">
         <v>283</v>
       </c>
@@ -11574,7 +11585,7 @@
       <c r="M26" s="8"/>
       <c r="N26" s="9"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A27" s="27" t="s">
         <v>314</v>
       </c>
@@ -11614,7 +11625,7 @@
       </c>
       <c r="N27" s="9"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A28" s="26" t="s">
         <v>315</v>
       </c>
@@ -11655,7 +11666,7 @@
       <c r="M28" s="8"/>
       <c r="N28" s="9"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A29" s="27" t="s">
         <v>316</v>
       </c>
@@ -11695,7 +11706,7 @@
       </c>
       <c r="N29" s="9"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A30" s="26" t="s">
         <v>284</v>
       </c>
@@ -11737,7 +11748,7 @@
       <c r="M30" s="8"/>
       <c r="N30" s="9"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A31" s="27" t="s">
         <v>322</v>
       </c>
@@ -11777,7 +11788,7 @@
       </c>
       <c r="N31" s="9"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A32" s="26" t="s">
         <v>287</v>
       </c>
@@ -11819,7 +11830,7 @@
       <c r="M32" s="8"/>
       <c r="N32" s="9"/>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A33" s="27" t="s">
         <v>320</v>
       </c>
@@ -11859,7 +11870,7 @@
       </c>
       <c r="N33" s="9"/>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A34" s="26" t="s">
         <v>367</v>
       </c>
@@ -11899,7 +11910,7 @@
       <c r="M34" s="8"/>
       <c r="N34" s="9"/>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A35" s="27" t="s">
         <v>370</v>
       </c>
@@ -11938,7 +11949,7 @@
       </c>
       <c r="N35" s="9"/>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A36" s="26" t="s">
         <v>288</v>
       </c>
@@ -11980,7 +11991,7 @@
       <c r="M36" s="8"/>
       <c r="N36" s="9"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A37" s="27" t="s">
         <v>289</v>
       </c>
@@ -12021,7 +12032,7 @@
       </c>
       <c r="N37" s="9"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A38" s="26" t="s">
         <v>373</v>
       </c>
@@ -12061,7 +12072,7 @@
       <c r="M38" s="8"/>
       <c r="N38" s="9"/>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A39" s="27" t="s">
         <v>355</v>
       </c>
@@ -12100,7 +12111,7 @@
       </c>
       <c r="N39" s="9"/>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A40" s="26" t="s">
         <v>290</v>
       </c>
@@ -12142,7 +12153,7 @@
       <c r="M40" s="8"/>
       <c r="N40" s="9"/>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A41" s="27" t="s">
         <v>353</v>
       </c>
@@ -12181,7 +12192,7 @@
       </c>
       <c r="N41" s="9"/>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A42" s="26" t="s">
         <v>291</v>
       </c>
@@ -12223,7 +12234,7 @@
       <c r="M42" s="8"/>
       <c r="N42" s="9"/>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A43" s="27" t="s">
         <v>346</v>
       </c>
@@ -12262,7 +12273,7 @@
       </c>
       <c r="N43" s="9"/>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A44" s="26" t="s">
         <v>384</v>
       </c>
@@ -12302,7 +12313,7 @@
       <c r="M44" s="8"/>
       <c r="N44" s="9"/>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A45" s="27" t="s">
         <v>383</v>
       </c>
@@ -12341,7 +12352,7 @@
       </c>
       <c r="N45" s="9"/>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A46" s="26" t="s">
         <v>354</v>
       </c>
@@ -12381,7 +12392,7 @@
       <c r="M46" s="8"/>
       <c r="N46" s="9"/>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A47" s="27" t="s">
         <v>362</v>
       </c>
@@ -12420,7 +12431,7 @@
       </c>
       <c r="N47" s="9"/>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A48" s="26" t="s">
         <v>321</v>
       </c>
@@ -12461,7 +12472,7 @@
       <c r="M48" s="8"/>
       <c r="N48" s="9"/>
     </row>
-    <row r="49" spans="1:230" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:230" x14ac:dyDescent="0.45">
       <c r="A49" s="27" t="s">
         <v>349</v>
       </c>
@@ -12500,7 +12511,7 @@
       </c>
       <c r="N49" s="9"/>
     </row>
-    <row r="50" spans="1:230" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:230" x14ac:dyDescent="0.45">
       <c r="A50" s="26" t="s">
         <v>379</v>
       </c>
@@ -12540,7 +12551,7 @@
       <c r="M50" s="8"/>
       <c r="N50" s="9"/>
     </row>
-    <row r="51" spans="1:230" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:230" x14ac:dyDescent="0.45">
       <c r="A51" s="27" t="s">
         <v>292</v>
       </c>
@@ -12581,7 +12592,7 @@
       </c>
       <c r="N51" s="9"/>
     </row>
-    <row r="52" spans="1:230" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:230" x14ac:dyDescent="0.45">
       <c r="A52" s="26" t="s">
         <v>365</v>
       </c>
@@ -12621,7 +12632,7 @@
       <c r="M52" s="8"/>
       <c r="N52" s="9"/>
     </row>
-    <row r="53" spans="1:230" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:230" x14ac:dyDescent="0.45">
       <c r="A53" s="27" t="s">
         <v>344</v>
       </c>
@@ -12660,7 +12671,7 @@
       </c>
       <c r="N53" s="9"/>
     </row>
-    <row r="54" spans="1:230" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:230" x14ac:dyDescent="0.45">
       <c r="A54" s="26" t="s">
         <v>325</v>
       </c>
@@ -12701,7 +12712,7 @@
       <c r="M54" s="8"/>
       <c r="N54" s="9"/>
     </row>
-    <row r="55" spans="1:230" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:230" x14ac:dyDescent="0.45">
       <c r="A55" s="27" t="s">
         <v>293</v>
       </c>
@@ -12742,7 +12753,7 @@
       </c>
       <c r="N55" s="9"/>
     </row>
-    <row r="56" spans="1:230" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:230" x14ac:dyDescent="0.45">
       <c r="A56" s="26" t="s">
         <v>348</v>
       </c>
@@ -12782,7 +12793,7 @@
       <c r="M56" s="8"/>
       <c r="N56" s="9"/>
     </row>
-    <row r="57" spans="1:230" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:230" x14ac:dyDescent="0.45">
       <c r="A57" s="27" t="s">
         <v>294</v>
       </c>
@@ -12823,7 +12834,7 @@
       </c>
       <c r="N57" s="9"/>
     </row>
-    <row r="58" spans="1:230" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:230" x14ac:dyDescent="0.45">
       <c r="A58" s="26" t="s">
         <v>295</v>
       </c>
@@ -12865,7 +12876,7 @@
       <c r="M58" s="8"/>
       <c r="N58" s="9"/>
     </row>
-    <row r="59" spans="1:230" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:230" x14ac:dyDescent="0.45">
       <c r="A59" s="27" t="s">
         <v>296</v>
       </c>
@@ -12906,7 +12917,7 @@
       </c>
       <c r="N59" s="9"/>
     </row>
-    <row r="60" spans="1:230" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:230" x14ac:dyDescent="0.45">
       <c r="A60" s="26" t="s">
         <v>368</v>
       </c>
@@ -12946,7 +12957,7 @@
       <c r="M60" s="8"/>
       <c r="N60" s="9"/>
     </row>
-    <row r="61" spans="1:230" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:230" x14ac:dyDescent="0.45">
       <c r="A61" s="27" t="s">
         <v>326</v>
       </c>
@@ -12986,7 +12997,7 @@
       </c>
       <c r="N61" s="9"/>
     </row>
-    <row r="62" spans="1:230" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:230" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A62" s="26" t="s">
         <v>351</v>
       </c>
@@ -13241,7 +13252,7 @@
       <c r="HU62" s="10"/>
       <c r="HV62" s="10"/>
     </row>
-    <row r="63" spans="1:230" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:230" x14ac:dyDescent="0.45">
       <c r="A63" s="27" t="s">
         <v>327</v>
       </c>
@@ -13281,7 +13292,7 @@
       </c>
       <c r="N63" s="9"/>
     </row>
-    <row r="64" spans="1:230" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:230" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A64" s="26" t="s">
         <v>387</v>
       </c>
@@ -13536,7 +13547,7 @@
       <c r="HU64" s="10"/>
       <c r="HV64" s="10"/>
     </row>
-    <row r="65" spans="1:230" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:230" x14ac:dyDescent="0.45">
       <c r="A65" s="27" t="s">
         <v>323</v>
       </c>
@@ -13576,7 +13587,7 @@
       </c>
       <c r="N65" s="9"/>
     </row>
-    <row r="66" spans="1:230" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:230" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A66" s="26" t="s">
         <v>324</v>
       </c>
@@ -13832,7 +13843,7 @@
       <c r="HU66" s="10"/>
       <c r="HV66" s="10"/>
     </row>
-    <row r="67" spans="1:230" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:230" x14ac:dyDescent="0.45">
       <c r="A67" s="27" t="s">
         <v>345</v>
       </c>
@@ -13871,7 +13882,7 @@
       </c>
       <c r="N67" s="9"/>
     </row>
-    <row r="68" spans="1:230" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:230" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A68" s="26" t="s">
         <v>297</v>
       </c>
@@ -14128,7 +14139,7 @@
       <c r="HU68" s="10"/>
       <c r="HV68" s="10"/>
     </row>
-    <row r="69" spans="1:230" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:230" x14ac:dyDescent="0.45">
       <c r="A69" s="27" t="s">
         <v>385</v>
       </c>
@@ -14167,7 +14178,7 @@
       </c>
       <c r="N69" s="9"/>
     </row>
-    <row r="70" spans="1:230" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:230" x14ac:dyDescent="0.45">
       <c r="A70" s="26" t="s">
         <v>374</v>
       </c>
@@ -14207,7 +14218,7 @@
       <c r="M70" s="8"/>
       <c r="N70" s="9"/>
     </row>
-    <row r="71" spans="1:230" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:230" x14ac:dyDescent="0.45">
       <c r="A71" s="27" t="s">
         <v>372</v>
       </c>
@@ -14250,7 +14261,7 @@
       <c r="R71" s="13"/>
       <c r="S71" s="13"/>
     </row>
-    <row r="72" spans="1:230" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:230" x14ac:dyDescent="0.45">
       <c r="A72" s="26" t="s">
         <v>298</v>
       </c>
@@ -14294,7 +14305,7 @@
       <c r="O72" s="15"/>
       <c r="Q72" s="16"/>
     </row>
-    <row r="73" spans="1:230" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:230" x14ac:dyDescent="0.45">
       <c r="A73" s="27" t="s">
         <v>299</v>
       </c>
@@ -14339,7 +14350,7 @@
       <c r="R73" s="15"/>
       <c r="S73" s="15"/>
     </row>
-    <row r="74" spans="1:230" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:230" x14ac:dyDescent="0.45">
       <c r="A74" s="26" t="s">
         <v>300</v>
       </c>
@@ -14383,7 +14394,7 @@
       <c r="O74" s="15"/>
       <c r="P74" s="15"/>
     </row>
-    <row r="75" spans="1:230" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:230" x14ac:dyDescent="0.45">
       <c r="A75" s="27" t="s">
         <v>347</v>
       </c>
@@ -14422,7 +14433,7 @@
       </c>
       <c r="N75" s="9"/>
     </row>
-    <row r="76" spans="1:230" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:230" x14ac:dyDescent="0.45">
       <c r="A76" s="26" t="s">
         <v>301</v>
       </c>
@@ -14464,7 +14475,7 @@
       <c r="M76" s="8"/>
       <c r="N76" s="9"/>
     </row>
-    <row r="77" spans="1:230" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:230" x14ac:dyDescent="0.45">
       <c r="A77" s="27" t="s">
         <v>382</v>
       </c>
@@ -14503,7 +14514,7 @@
       </c>
       <c r="N77" s="9"/>
     </row>
-    <row r="78" spans="1:230" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:230" x14ac:dyDescent="0.45">
       <c r="A78" s="26" t="s">
         <v>330</v>
       </c>
@@ -14544,7 +14555,7 @@
       <c r="M78" s="8"/>
       <c r="N78" s="9"/>
     </row>
-    <row r="79" spans="1:230" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:230" x14ac:dyDescent="0.45">
       <c r="A79" s="27" t="s">
         <v>361</v>
       </c>
@@ -14583,7 +14594,7 @@
       </c>
       <c r="N79" s="9"/>
     </row>
-    <row r="80" spans="1:230" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:230" x14ac:dyDescent="0.45">
       <c r="A80" s="26" t="s">
         <v>360</v>
       </c>
@@ -14623,7 +14634,7 @@
       <c r="M80" s="8"/>
       <c r="N80" s="9"/>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A81" s="27" t="s">
         <v>328</v>
       </c>
@@ -14663,7 +14674,7 @@
       </c>
       <c r="N81" s="9"/>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A82" s="26" t="s">
         <v>380</v>
       </c>
@@ -14703,7 +14714,7 @@
       <c r="M82" s="8"/>
       <c r="N82" s="9"/>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A83" s="27" t="s">
         <v>329</v>
       </c>
@@ -14743,7 +14754,7 @@
       </c>
       <c r="N83" s="9"/>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A84" s="26" t="s">
         <v>302</v>
       </c>
@@ -14785,7 +14796,7 @@
       <c r="M84" s="8"/>
       <c r="N84" s="9"/>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A85" s="27" t="s">
         <v>303</v>
       </c>
@@ -14826,7 +14837,7 @@
       </c>
       <c r="N85" s="9"/>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A86" s="26" t="s">
         <v>304</v>
       </c>
@@ -14868,7 +14879,7 @@
       <c r="M86" s="8"/>
       <c r="N86" s="9"/>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A87" s="27" t="s">
         <v>371</v>
       </c>
@@ -14907,7 +14918,7 @@
       </c>
       <c r="N87" s="9"/>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A88" s="26" t="s">
         <v>332</v>
       </c>
@@ -14948,7 +14959,7 @@
       <c r="M88" s="8"/>
       <c r="N88" s="9"/>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A89" s="27" t="s">
         <v>333</v>
       </c>
@@ -14988,7 +14999,7 @@
       </c>
       <c r="N89" s="9"/>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A90" s="26" t="s">
         <v>305</v>
       </c>
@@ -15030,7 +15041,7 @@
       <c r="M90" s="8"/>
       <c r="N90" s="9"/>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A91" s="27" t="s">
         <v>334</v>
       </c>
@@ -15070,7 +15081,7 @@
       </c>
       <c r="N91" s="9"/>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A92" s="26" t="s">
         <v>376</v>
       </c>
@@ -15110,7 +15121,7 @@
       <c r="M92" s="8"/>
       <c r="N92" s="9"/>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A93" s="27" t="s">
         <v>343</v>
       </c>
@@ -15149,7 +15160,7 @@
       </c>
       <c r="N93" s="9"/>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A94" s="26" t="s">
         <v>331</v>
       </c>
@@ -15190,7 +15201,7 @@
       <c r="M94" s="8"/>
       <c r="N94" s="9"/>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A95" s="27" t="s">
         <v>375</v>
       </c>
@@ -15229,7 +15240,7 @@
       </c>
       <c r="N95" s="9"/>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A96" s="26" t="s">
         <v>350</v>
       </c>
@@ -15269,7 +15280,7 @@
       <c r="M96" s="8"/>
       <c r="N96" s="9"/>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A97" s="27" t="s">
         <v>336</v>
       </c>
@@ -15309,7 +15320,7 @@
       </c>
       <c r="N97" s="9"/>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A98" s="26" t="s">
         <v>337</v>
       </c>
@@ -15340,7 +15351,7 @@
       <c r="M98" s="8"/>
       <c r="N98" s="9"/>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A99" s="27" t="s">
         <v>306</v>
       </c>
@@ -15381,7 +15392,7 @@
       </c>
       <c r="N99" s="9"/>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A100" s="26" t="s">
         <v>307</v>
       </c>
@@ -15423,7 +15434,7 @@
       <c r="M100" s="8"/>
       <c r="N100" s="9"/>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A101" s="27" t="s">
         <v>357</v>
       </c>
@@ -15462,7 +15473,7 @@
       </c>
       <c r="N101" s="9"/>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A102" s="26" t="s">
         <v>338</v>
       </c>
@@ -15503,7 +15514,7 @@
       <c r="M102" s="8"/>
       <c r="N102" s="9"/>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A103" s="27" t="s">
         <v>378</v>
       </c>
@@ -15542,7 +15553,7 @@
       </c>
       <c r="N103" s="9"/>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A104" s="26" t="s">
         <v>364</v>
       </c>
@@ -15582,7 +15593,7 @@
       <c r="M104" s="8"/>
       <c r="N104" s="9"/>
     </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A105" s="27" t="s">
         <v>335</v>
       </c>
@@ -15622,7 +15633,7 @@
       </c>
       <c r="N105" s="9"/>
     </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A106" s="26" t="s">
         <v>308</v>
       </c>
@@ -15664,7 +15675,7 @@
       <c r="M106" s="8"/>
       <c r="N106" s="9"/>
     </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A107" s="27" t="s">
         <v>340</v>
       </c>
@@ -15704,7 +15715,7 @@
       </c>
       <c r="N107" s="9"/>
     </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A108" s="26" t="s">
         <v>341</v>
       </c>
@@ -15745,7 +15756,7 @@
       <c r="M108" s="8"/>
       <c r="N108" s="9"/>
     </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A109" s="27" t="s">
         <v>339</v>
       </c>
@@ -15785,7 +15796,7 @@
       </c>
       <c r="N109" s="9"/>
     </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A110" s="26" t="s">
         <v>369</v>
       </c>
@@ -15825,7 +15836,7 @@
       <c r="M110" s="8"/>
       <c r="N110" s="9"/>
     </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A111" s="9"/>
       <c r="B111" s="9"/>
       <c r="C111" s="9"/>
@@ -15841,7 +15852,7 @@
       <c r="M111" s="9"/>
       <c r="N111" s="9"/>
     </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A112" s="10" t="s">
         <v>309</v>
       </c>
@@ -15850,16 +15861,16 @@
       </c>
       <c r="N112" s="9"/>
     </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A113" s="27"/>
       <c r="N113" s="9"/>
     </row>
-    <row r="116" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A116" s="18"/>
       <c r="B116" s="18"/>
     </row>
   </sheetData>
-  <sortState ref="A6:G110">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:G110">
     <sortCondition ref="A5"/>
   </sortState>
   <mergeCells count="1">

</xml_diff>